<commit_message>
Worked on MCDM problems
</commit_message>
<xml_diff>
--- a/Python Data Analytics/Jupyter Notebooks/outputelectre.xlsx
+++ b/Python Data Analytics/Jupyter Notebooks/outputelectre.xlsx
@@ -7,21 +7,21 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Global_Concordance" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Global Concordance" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Credibility" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Discordance_SJR-index" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Discordance_Cite Score" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Discordance_H-index" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Discordance_Best Subject Rank" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Discordance_Total Docs" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Discordance_Total Docs 3y" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Discordance_Total Refs" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Discordance_Total Cites 3y" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Discordance_Citable Docs 3y" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Discordance_Cites per Doc 2y" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Discordance_Refs per Doc" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="Discordance_Coverage" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="Final_Ranking" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Discordance SJR-index" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Discordance Cite Score" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Discordance H-index" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Discordance Best Subject Rank" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Discordance Total Docs" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Discordance Total Docs 3y" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Discordance Total Refs" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Discordance Total Cites 3y" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Discordance Citable Docs 3y" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Discordance Cites per Doc 2y" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Discordance Refs per Doc" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Discordance Coverage" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Final Ranking" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>